<commit_message>
Remove top-level report artifacts; keep outputs in output/
</commit_message>
<xml_diff>
--- a/data/forces.xlsx
+++ b/data/forces.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,37 +424,1129 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>pos</t>
+          <t>X</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>mag</t>
+          <t>Shear force</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Bending Moment</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>500</v>
+        <v>5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3</v>
+        <v>0.1</v>
       </c>
       <c r="B3" t="n">
-        <v>800</v>
+        <v>4.9</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.4975</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1.4775</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1.96</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>2.4375</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="B8" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2.910000000000001</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>0.7000000000000001</v>
+      </c>
+      <c r="B9" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="C9" t="n">
+        <v>3.3775</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="C10" t="n">
+        <v>3.84</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="C11" t="n">
+        <v>4.2975</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1</v>
+      </c>
+      <c r="B12" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" t="n">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="B13" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="C13" t="n">
+        <v>5.1975</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="B14" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="C14" t="n">
+        <v>5.640000000000001</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="B15" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="C15" t="n">
+        <v>6.0775</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="B16" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="C16" t="n">
+        <v>6.510000000000001</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="B17" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="C17" t="n">
+        <v>6.9375</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="B18" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="C18" t="n">
+        <v>7.359999999999999</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="B19" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="C19" t="n">
+        <v>7.7775</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="B20" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="C20" t="n">
+        <v>8.19</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="B21" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="C21" t="n">
+        <v>8.5975</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>2</v>
+      </c>
+      <c r="B22" t="n">
+        <v>3</v>
+      </c>
+      <c r="C22" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="B23" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="C23" t="n">
+        <v>9.397500000000001</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="B24" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="C24" t="n">
+        <v>9.789999999999999</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="B25" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="C25" t="n">
+        <v>10.1775</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="B26" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="C26" t="n">
+        <v>10.56</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="B27" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="C27" t="n">
+        <v>10.9375</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="B28" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="C28" t="n">
+        <v>11.31</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="B29" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="C29" t="n">
+        <v>11.6775</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="B30" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="C30" t="n">
+        <v>12.04</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="B31" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="C31" t="n">
+        <v>12.3975</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>3</v>
+      </c>
+      <c r="B32" t="n">
+        <v>2</v>
+      </c>
+      <c r="C32" t="n">
+        <v>12.75</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="B33" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="C33" t="n">
+        <v>13.0975</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="B34" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="C34" t="n">
+        <v>13.44</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="B35" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="C35" t="n">
+        <v>13.7775</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="B36" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="C36" t="n">
+        <v>14.11</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="B37" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="C37" t="n">
+        <v>14.4375</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="B38" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="C38" t="n">
+        <v>14.76</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="B39" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="C39" t="n">
+        <v>15.0775</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="B40" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="C40" t="n">
+        <v>15.39</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="B41" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="C41" t="n">
+        <v>15.6975</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>4</v>
+      </c>
+      <c r="B42" t="n">
+        <v>1</v>
+      </c>
+      <c r="C42" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>4.100000000000001</v>
+      </c>
+      <c r="B43" t="n">
+        <v>0.8999999999999995</v>
+      </c>
+      <c r="C43" t="n">
+        <v>16.2975</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="B44" t="n">
+        <v>0.7999999999999998</v>
+      </c>
+      <c r="C44" t="n">
+        <v>16.59</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="B45" t="n">
+        <v>0.7000000000000002</v>
+      </c>
+      <c r="C45" t="n">
+        <v>16.8775</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="B46" t="n">
+        <v>0.5999999999999996</v>
+      </c>
+      <c r="C46" t="n">
+        <v>17.16</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="B47" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C47" t="n">
+        <v>17.4375</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>4.600000000000001</v>
+      </c>
+      <c r="B48" t="n">
+        <v>0.3999999999999995</v>
+      </c>
+      <c r="C48" t="n">
+        <v>17.71</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="B49" t="n">
+        <v>0.2999999999999998</v>
+      </c>
+      <c r="C49" t="n">
+        <v>17.9775</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>4.800000000000001</v>
+      </c>
+      <c r="B50" t="n">
+        <v>0.1999999999999993</v>
+      </c>
+      <c r="C50" t="n">
+        <v>18.24</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="B51" t="n">
+        <v>0.09999999999999964</v>
+      </c>
+      <c r="C51" t="n">
+        <v>18.4975</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>5</v>
+      </c>
+      <c r="B52" t="n">
+        <v>0</v>
+      </c>
+      <c r="C52" t="n">
+        <v>18.75</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>5.100000000000001</v>
+      </c>
+      <c r="B53" t="n">
+        <v>-0.1000000000000005</v>
+      </c>
+      <c r="C53" t="n">
+        <v>18.9975</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="B54" t="n">
+        <v>-0.2000000000000002</v>
+      </c>
+      <c r="C54" t="n">
+        <v>19.24</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>5.300000000000001</v>
+      </c>
+      <c r="B55" t="n">
+        <v>-0.3000000000000007</v>
+      </c>
+      <c r="C55" t="n">
+        <v>19.4775</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="B56" t="n">
+        <v>-0.4000000000000004</v>
+      </c>
+      <c r="C56" t="n">
+        <v>19.71</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="B57" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="C57" t="n">
+        <v>19.9375</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>5.600000000000001</v>
+      </c>
+      <c r="B58" t="n">
+        <v>-0.6000000000000005</v>
+      </c>
+      <c r="C58" t="n">
+        <v>20.16</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="B59" t="n">
+        <v>-0.7000000000000002</v>
+      </c>
+      <c r="C59" t="n">
+        <v>20.3775</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>5.800000000000001</v>
+      </c>
+      <c r="B60" t="n">
+        <v>-0.8000000000000007</v>
+      </c>
+      <c r="C60" t="n">
+        <v>20.59</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="B61" t="n">
+        <v>-0.9000000000000004</v>
+      </c>
+      <c r="C61" t="n">
+        <v>20.7975</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
         <v>6</v>
       </c>
-      <c r="B4" t="n">
-        <v>300</v>
+      <c r="B62" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C62" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>6.100000000000001</v>
+      </c>
+      <c r="B63" t="n">
+        <v>-1.100000000000001</v>
+      </c>
+      <c r="C63" t="n">
+        <v>21.1975</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="B64" t="n">
+        <v>-1.2</v>
+      </c>
+      <c r="C64" t="n">
+        <v>21.39</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>6.300000000000001</v>
+      </c>
+      <c r="B65" t="n">
+        <v>-1.300000000000001</v>
+      </c>
+      <c r="C65" t="n">
+        <v>21.5775</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="B66" t="n">
+        <v>-1.4</v>
+      </c>
+      <c r="C66" t="n">
+        <v>21.76</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="B67" t="n">
+        <v>-1.5</v>
+      </c>
+      <c r="C67" t="n">
+        <v>21.9375</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>6.600000000000001</v>
+      </c>
+      <c r="B68" t="n">
+        <v>-1.600000000000001</v>
+      </c>
+      <c r="C68" t="n">
+        <v>22.11</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="B69" t="n">
+        <v>-1.7</v>
+      </c>
+      <c r="C69" t="n">
+        <v>22.2775</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>6.800000000000001</v>
+      </c>
+      <c r="B70" t="n">
+        <v>-1.800000000000001</v>
+      </c>
+      <c r="C70" t="n">
+        <v>22.44</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="B71" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="C71" t="n">
+        <v>22.5975</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>7</v>
+      </c>
+      <c r="B72" t="n">
+        <v>-2</v>
+      </c>
+      <c r="C72" t="n">
+        <v>22.75</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>7.100000000000001</v>
+      </c>
+      <c r="B73" t="n">
+        <v>-2.100000000000001</v>
+      </c>
+      <c r="C73" t="n">
+        <v>22.8975</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="B74" t="n">
+        <v>-2.2</v>
+      </c>
+      <c r="C74" t="n">
+        <v>23.04</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>7.300000000000001</v>
+      </c>
+      <c r="B75" t="n">
+        <v>-2.300000000000001</v>
+      </c>
+      <c r="C75" t="n">
+        <v>23.17749999999999</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="B76" t="n">
+        <v>-2.4</v>
+      </c>
+      <c r="C76" t="n">
+        <v>23.31</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="B77" t="n">
+        <v>-2.5</v>
+      </c>
+      <c r="C77" t="n">
+        <v>23.4375</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>7.600000000000001</v>
+      </c>
+      <c r="B78" t="n">
+        <v>-2.600000000000001</v>
+      </c>
+      <c r="C78" t="n">
+        <v>23.56</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>7.7</v>
+      </c>
+      <c r="B79" t="n">
+        <v>-2.7</v>
+      </c>
+      <c r="C79" t="n">
+        <v>23.6775</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>7.800000000000001</v>
+      </c>
+      <c r="B80" t="n">
+        <v>-2.800000000000001</v>
+      </c>
+      <c r="C80" t="n">
+        <v>23.79</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="B81" t="n">
+        <v>-2.9</v>
+      </c>
+      <c r="C81" t="n">
+        <v>23.8975</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>8</v>
+      </c>
+      <c r="B82" t="n">
+        <v>-3</v>
+      </c>
+      <c r="C82" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="B83" t="n">
+        <v>-3.1</v>
+      </c>
+      <c r="C83" t="n">
+        <v>24.0975</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>8.200000000000001</v>
+      </c>
+      <c r="B84" t="n">
+        <v>-3.200000000000001</v>
+      </c>
+      <c r="C84" t="n">
+        <v>24.19</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>8.300000000000001</v>
+      </c>
+      <c r="B85" t="n">
+        <v>-3.300000000000001</v>
+      </c>
+      <c r="C85" t="n">
+        <v>24.2775</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="B86" t="n">
+        <v>-3.4</v>
+      </c>
+      <c r="C86" t="n">
+        <v>24.36</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="B87" t="n">
+        <v>-3.5</v>
+      </c>
+      <c r="C87" t="n">
+        <v>24.4375</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="B88" t="n">
+        <v>-3.6</v>
+      </c>
+      <c r="C88" t="n">
+        <v>24.51</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>8.700000000000001</v>
+      </c>
+      <c r="B89" t="n">
+        <v>-3.700000000000001</v>
+      </c>
+      <c r="C89" t="n">
+        <v>24.5775</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>8.800000000000001</v>
+      </c>
+      <c r="B90" t="n">
+        <v>-3.800000000000001</v>
+      </c>
+      <c r="C90" t="n">
+        <v>24.64</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="B91" t="n">
+        <v>-3.9</v>
+      </c>
+      <c r="C91" t="n">
+        <v>24.6975</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>9</v>
+      </c>
+      <c r="B92" t="n">
+        <v>-4</v>
+      </c>
+      <c r="C92" t="n">
+        <v>24.75</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>9.1</v>
+      </c>
+      <c r="B93" t="n">
+        <v>-4.1</v>
+      </c>
+      <c r="C93" t="n">
+        <v>24.7975</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>9.200000000000001</v>
+      </c>
+      <c r="B94" t="n">
+        <v>-4.200000000000001</v>
+      </c>
+      <c r="C94" t="n">
+        <v>24.84</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>9.300000000000001</v>
+      </c>
+      <c r="B95" t="n">
+        <v>-4.300000000000001</v>
+      </c>
+      <c r="C95" t="n">
+        <v>24.8775</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>9.4</v>
+      </c>
+      <c r="B96" t="n">
+        <v>-4.4</v>
+      </c>
+      <c r="C96" t="n">
+        <v>24.91</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="B97" t="n">
+        <v>-4.5</v>
+      </c>
+      <c r="C97" t="n">
+        <v>24.9375</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>9.600000000000001</v>
+      </c>
+      <c r="B98" t="n">
+        <v>-4.600000000000001</v>
+      </c>
+      <c r="C98" t="n">
+        <v>24.96</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>9.700000000000001</v>
+      </c>
+      <c r="B99" t="n">
+        <v>-4.700000000000001</v>
+      </c>
+      <c r="C99" t="n">
+        <v>24.9775</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>9.800000000000001</v>
+      </c>
+      <c r="B100" t="n">
+        <v>-4.800000000000001</v>
+      </c>
+      <c r="C100" t="n">
+        <v>24.98999999999999</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>9.9</v>
+      </c>
+      <c r="B101" t="n">
+        <v>-4.9</v>
+      </c>
+      <c r="C101" t="n">
+        <v>24.9975</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>10</v>
+      </c>
+      <c r="B102" t="n">
+        <v>-5</v>
+      </c>
+      <c r="C102" t="n">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>